<commit_message>
add identifiers and terms (organs)
</commit_message>
<xml_diff>
--- a/annotation.xlsx
+++ b/annotation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\keeran\functional-connectivity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{963CC90F-4E43-4AE7-869F-3AE5395E42CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1883CB5D-8374-4481-BDF6-62EC62AF46B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="7275" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="10080" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OrganSystems" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3810" uniqueCount="901">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3807" uniqueCount="965">
   <si>
     <t>Organ System Name</t>
   </si>
@@ -2514,9 +2514,6 @@
     <t>taste</t>
   </si>
   <si>
-    <t>testes</t>
-  </si>
-  <si>
     <t>thigh-musc</t>
   </si>
   <si>
@@ -2758,6 +2755,201 @@
   </si>
   <si>
     <t>ILX:52623</t>
+  </si>
+  <si>
+    <t>ILX:0744822</t>
+  </si>
+  <si>
+    <t>UBERON:0003716</t>
+  </si>
+  <si>
+    <t>UBERON:0001584</t>
+  </si>
+  <si>
+    <t>UBERON:0001383</t>
+  </si>
+  <si>
+    <t>ILX:0741471</t>
+  </si>
+  <si>
+    <t>UBERON:0003721</t>
+  </si>
+  <si>
+    <t>UBERON:0002107</t>
+  </si>
+  <si>
+    <t>UBERON:0004907</t>
+  </si>
+  <si>
+    <t>UBERON:0018683</t>
+  </si>
+  <si>
+    <t>UBERON:0002048</t>
+  </si>
+  <si>
+    <t>UBERON:0000375</t>
+  </si>
+  <si>
+    <t>UBERON:0000377</t>
+  </si>
+  <si>
+    <t>ILX:0793557</t>
+  </si>
+  <si>
+    <t>UBERON:0001896</t>
+  </si>
+  <si>
+    <t>UBERON:0001891</t>
+  </si>
+  <si>
+    <t>UBERON:0003963</t>
+  </si>
+  <si>
+    <t>ILX:0745944</t>
+  </si>
+  <si>
+    <t>UBERON:0001264</t>
+  </si>
+  <si>
+    <t>UBERON:0001807</t>
+  </si>
+  <si>
+    <t>UBERON:0016508</t>
+  </si>
+  <si>
+    <t>UBERON:0018675</t>
+  </si>
+  <si>
+    <t>UBERON:0000989</t>
+  </si>
+  <si>
+    <t>UBERON:0019197</t>
+  </si>
+  <si>
+    <t>UBERON:0011325</t>
+  </si>
+  <si>
+    <t>ILX:0743160</t>
+  </si>
+  <si>
+    <t>UBERON:0006562</t>
+  </si>
+  <si>
+    <t>UBERON:0000988</t>
+  </si>
+  <si>
+    <t>ILX:0745275</t>
+  </si>
+  <si>
+    <t>UBERON:0003962</t>
+  </si>
+  <si>
+    <t>UBERON:0011390</t>
+  </si>
+  <si>
+    <t>UBERON:0002009</t>
+  </si>
+  <si>
+    <t>FMA:52622</t>
+  </si>
+  <si>
+    <t>ILX:0743107</t>
+  </si>
+  <si>
+    <t>UBERON:0018676</t>
+  </si>
+  <si>
+    <t>UBERON:0001534</t>
+  </si>
+  <si>
+    <t>UBERON:0018684</t>
+  </si>
+  <si>
+    <t>ILX:0110617</t>
+  </si>
+  <si>
+    <t>UBERON:0002240</t>
+  </si>
+  <si>
+    <t>UBERON:0002106</t>
+  </si>
+  <si>
+    <t>UBERON:0000945</t>
+  </si>
+  <si>
+    <t>UBERON:0002059</t>
+  </si>
+  <si>
+    <t>UBERON:0002013</t>
+  </si>
+  <si>
+    <t>UBERON:0006564</t>
+  </si>
+  <si>
+    <t>UBERON:00113263</t>
+  </si>
+  <si>
+    <t>ILX:0745792</t>
+  </si>
+  <si>
+    <t>testis</t>
+  </si>
+  <si>
+    <t>UBERON:0000473</t>
+  </si>
+  <si>
+    <t>UBERON:0001515</t>
+  </si>
+  <si>
+    <t>ILX:0744319</t>
+  </si>
+  <si>
+    <t>UBERON:0001675</t>
+  </si>
+  <si>
+    <t>UBERON:0001482</t>
+  </si>
+  <si>
+    <t>UBERON:0036216</t>
+  </si>
+  <si>
+    <t>UBERON:0000056</t>
+  </si>
+  <si>
+    <t>UBERON:0000057</t>
+  </si>
+  <si>
+    <t>UBERON:0000995</t>
+  </si>
+  <si>
+    <t>UBERON:0001645</t>
+  </si>
+  <si>
+    <t>UBERON:0001647</t>
+  </si>
+  <si>
+    <t>UBERON:0000996</t>
+  </si>
+  <si>
+    <t>UBERON:0002824</t>
+  </si>
+  <si>
+    <t>UBERON:0003723</t>
+  </si>
+  <si>
+    <t>ILX:0741477</t>
+  </si>
+  <si>
+    <t>ILX:0112501</t>
+  </si>
+  <si>
+    <t>UBERON:0001759</t>
+  </si>
+  <si>
+    <t>FMA:6248</t>
+  </si>
+  <si>
+    <t>ILX:0743680</t>
   </si>
 </sst>
 </file>
@@ -3438,8 +3630,8 @@
   <dimension ref="A1:G258"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C111" sqref="C111"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C259" sqref="C259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3696,7 +3888,7 @@
         <v>639</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>7</v>
@@ -3713,7 +3905,7 @@
         <v>640</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>7</v>
@@ -3781,7 +3973,7 @@
         <v>631</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>10</v>
@@ -3798,7 +3990,7 @@
         <v>651</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>19</v>
@@ -3815,7 +4007,7 @@
         <v>650</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>7</v>
@@ -3846,7 +4038,7 @@
         <v>652</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>9</v>
@@ -3863,7 +4055,7 @@
         <v>644</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>53</v>
@@ -3877,7 +4069,7 @@
         <v>653</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>7</v>
@@ -3908,7 +4100,7 @@
         <v>654</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>7</v>
@@ -3925,7 +4117,7 @@
         <v>655</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>7</v>
@@ -3976,7 +4168,7 @@
         <v>658</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>7</v>
@@ -3993,7 +4185,7 @@
         <v>622</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>7</v>
@@ -4010,7 +4202,7 @@
         <v>659</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>9</v>
@@ -4027,7 +4219,7 @@
         <v>660</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>7</v>
@@ -4044,7 +4236,7 @@
         <v>661</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>7</v>
@@ -4061,7 +4253,7 @@
         <v>662</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>7</v>
@@ -4078,7 +4270,7 @@
         <v>622</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>7</v>
@@ -4095,7 +4287,7 @@
         <v>663</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>7</v>
@@ -4112,7 +4304,7 @@
         <v>664</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>7</v>
@@ -4126,10 +4318,10 @@
         <v>71</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>7</v>
@@ -4231,7 +4423,7 @@
         <v>646</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>9</v>
@@ -4248,7 +4440,7 @@
         <v>78</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>7</v>
@@ -4276,7 +4468,7 @@
         <v>80</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>7</v>
@@ -4293,7 +4485,7 @@
         <v>633</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>9</v>
@@ -4310,7 +4502,7 @@
         <v>637</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>9</v>
@@ -4327,7 +4519,7 @@
         <v>669</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>9</v>
@@ -4344,7 +4536,7 @@
         <v>670</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>9</v>
@@ -4361,7 +4553,7 @@
         <v>647</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>9</v>
@@ -4378,7 +4570,7 @@
         <v>671</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>7</v>
@@ -4412,7 +4604,7 @@
         <v>623</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>9</v>
@@ -4429,7 +4621,7 @@
         <v>673</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>9</v>
@@ -4446,7 +4638,7 @@
         <v>648</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>10</v>
@@ -4463,7 +4655,7 @@
         <v>674</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>7</v>
@@ -4514,7 +4706,7 @@
         <v>677</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>10</v>
@@ -4548,7 +4740,7 @@
         <v>762</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D66" s="5" t="s">
         <v>7</v>
@@ -4565,7 +4757,7 @@
         <v>679</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>16</v>
@@ -4650,7 +4842,7 @@
         <v>684</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>7</v>
@@ -4667,7 +4859,7 @@
         <v>685</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>7</v>
@@ -4684,7 +4876,7 @@
         <v>686</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>7</v>
@@ -4715,7 +4907,7 @@
         <v>688</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>7</v>
@@ -4783,7 +4975,7 @@
         <v>692</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>9</v>
@@ -4800,7 +4992,7 @@
         <v>693</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>7</v>
@@ -4817,7 +5009,7 @@
         <v>694</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>7</v>
@@ -4834,7 +5026,7 @@
         <v>695</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>9</v>
@@ -4851,7 +5043,7 @@
         <v>696</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>7</v>
@@ -4868,7 +5060,7 @@
         <v>697</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>7</v>
@@ -4885,7 +5077,7 @@
         <v>698</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>7</v>
@@ -4916,10 +5108,10 @@
         <v>121</v>
       </c>
       <c r="B88" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="C88" s="2" t="s">
         <v>892</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>893</v>
       </c>
       <c r="D88" s="5" t="s">
         <v>7</v>
@@ -4936,7 +5128,7 @@
         <v>700</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="G89" s="5" t="s">
         <v>116</v>
@@ -4950,7 +5142,7 @@
         <v>701</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="D90" s="5" t="s">
         <v>7</v>
@@ -4967,7 +5159,7 @@
         <v>702</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="D91" s="5" t="s">
         <v>9</v>
@@ -4984,7 +5176,7 @@
         <v>700</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="D92" s="5" t="s">
         <v>7</v>
@@ -5018,7 +5210,7 @@
         <v>705</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="D94" s="5" t="s">
         <v>9</v>
@@ -5035,7 +5227,7 @@
         <v>763</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="D95" s="5" t="s">
         <v>7</v>
@@ -5222,7 +5414,7 @@
         <v>706</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>19</v>
@@ -5290,7 +5482,7 @@
         <v>710</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>9</v>
@@ -5324,7 +5516,7 @@
         <v>712</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>5</v>
+        <v>900</v>
       </c>
       <c r="D112" s="5" t="s">
         <v>9</v>
@@ -5494,7 +5686,7 @@
         <v>717</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="D122" s="5" t="s">
         <v>7</v>
@@ -5579,7 +5771,7 @@
         <v>764</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>5</v>
+        <v>901</v>
       </c>
       <c r="D127" s="5" t="s">
         <v>7</v>
@@ -5613,7 +5805,7 @@
         <v>723</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>5</v>
+        <v>902</v>
       </c>
       <c r="D129" s="5" t="s">
         <v>9</v>
@@ -5630,7 +5822,7 @@
         <v>724</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>5</v>
+        <v>903</v>
       </c>
       <c r="D130" s="5" t="s">
         <v>14</v>
@@ -5647,7 +5839,7 @@
         <v>725</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>5</v>
+        <v>904</v>
       </c>
       <c r="D131" s="5" t="s">
         <v>7</v>
@@ -5664,7 +5856,7 @@
         <v>726</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="D132" s="5" t="s">
         <v>7</v>
@@ -5681,7 +5873,7 @@
         <v>727</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>5</v>
+        <v>905</v>
       </c>
       <c r="D133" s="5" t="s">
         <v>7</v>
@@ -5698,7 +5890,7 @@
         <v>728</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>5</v>
+        <v>906</v>
       </c>
       <c r="D134" s="5" t="s">
         <v>10</v>
@@ -5715,7 +5907,7 @@
         <v>729</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>5</v>
+        <v>907</v>
       </c>
       <c r="D135" s="5" t="s">
         <v>10</v>
@@ -5749,7 +5941,7 @@
         <v>731</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>5</v>
+        <v>908</v>
       </c>
       <c r="D137" s="5" t="s">
         <v>7</v>
@@ -5766,7 +5958,7 @@
         <v>732</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>5</v>
+        <v>909</v>
       </c>
       <c r="D138" s="5" t="s">
         <v>9</v>
@@ -5783,7 +5975,7 @@
         <v>733</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>5</v>
+        <v>910</v>
       </c>
       <c r="D139" s="5" t="s">
         <v>7</v>
@@ -5800,7 +5992,7 @@
         <v>734</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>5</v>
+        <v>911</v>
       </c>
       <c r="D140" s="5" t="s">
         <v>7</v>
@@ -5885,7 +6077,7 @@
         <v>739</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>5</v>
+        <v>912</v>
       </c>
       <c r="G145" s="5" t="s">
         <v>6</v>
@@ -5899,7 +6091,7 @@
         <v>740</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>5</v>
+        <v>913</v>
       </c>
       <c r="D146" s="5" t="s">
         <v>7</v>
@@ -5933,7 +6125,7 @@
         <v>742</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>5</v>
+        <v>914</v>
       </c>
       <c r="D148" s="5" t="s">
         <v>7</v>
@@ -6004,7 +6196,7 @@
         <v>746</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>5</v>
+        <v>915</v>
       </c>
       <c r="D152" s="5" t="s">
         <v>7</v>
@@ -6021,7 +6213,7 @@
         <v>747</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>5</v>
+        <v>916</v>
       </c>
       <c r="D153" s="5" t="s">
         <v>7</v>
@@ -6055,7 +6247,7 @@
         <v>749</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>5</v>
+        <v>917</v>
       </c>
       <c r="D155" s="5" t="s">
         <v>10</v>
@@ -6106,7 +6298,7 @@
         <v>752</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>5</v>
+        <v>918</v>
       </c>
       <c r="D158" s="5" t="s">
         <v>7</v>
@@ -6123,7 +6315,7 @@
         <v>753</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>5</v>
+        <v>919</v>
       </c>
       <c r="D159" s="5" t="s">
         <v>7</v>
@@ -6157,7 +6349,7 @@
         <v>755</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>5</v>
+        <v>920</v>
       </c>
       <c r="D161" s="5" t="s">
         <v>7</v>
@@ -6174,7 +6366,7 @@
         <v>755</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>5</v>
+        <v>920</v>
       </c>
       <c r="D162" s="5" t="s">
         <v>7</v>
@@ -6191,7 +6383,7 @@
         <v>756</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>5</v>
+        <v>921</v>
       </c>
       <c r="D163" s="5" t="s">
         <v>17</v>
@@ -6208,7 +6400,7 @@
         <v>757</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>5</v>
+        <v>922</v>
       </c>
       <c r="G164" s="5" t="s">
         <v>53</v>
@@ -6256,7 +6448,7 @@
         <v>765</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>5</v>
+        <v>923</v>
       </c>
       <c r="D167" s="5" t="s">
         <v>7</v>
@@ -6273,7 +6465,7 @@
         <v>761</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>5</v>
+        <v>924</v>
       </c>
       <c r="D168" s="5" t="s">
         <v>7</v>
@@ -6290,7 +6482,7 @@
         <v>767</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>5</v>
+        <v>925</v>
       </c>
       <c r="D169" s="5" t="s">
         <v>15</v>
@@ -6324,7 +6516,7 @@
         <v>766</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>5</v>
+        <v>926</v>
       </c>
       <c r="D171" s="5" t="s">
         <v>7</v>
@@ -6426,7 +6618,7 @@
         <v>773</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>5</v>
+        <v>927</v>
       </c>
       <c r="D177" s="5" t="s">
         <v>7</v>
@@ -6443,7 +6635,7 @@
         <v>774</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>5</v>
+        <v>928</v>
       </c>
       <c r="D178" s="5" t="s">
         <v>7</v>
@@ -6460,7 +6652,7 @@
         <v>775</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>5</v>
+        <v>929</v>
       </c>
       <c r="D179" s="5" t="s">
         <v>7</v>
@@ -6477,7 +6669,7 @@
         <v>776</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>5</v>
+        <v>930</v>
       </c>
       <c r="D180" s="5" t="s">
         <v>10</v>
@@ -6664,7 +6856,7 @@
         <v>787</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>5</v>
+        <v>931</v>
       </c>
       <c r="D191" s="5" t="s">
         <v>9</v>
@@ -6698,7 +6890,7 @@
         <v>789</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>5</v>
+        <v>900</v>
       </c>
       <c r="D193" s="5" t="s">
         <v>9</v>
@@ -6766,7 +6958,7 @@
         <v>797</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>5</v>
+        <v>932</v>
       </c>
       <c r="D197" s="5" t="s">
         <v>7</v>
@@ -6783,7 +6975,7 @@
         <v>798</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>5</v>
+        <v>933</v>
       </c>
       <c r="G198" s="5" t="s">
         <v>116</v>
@@ -6864,9 +7056,6 @@
       <c r="B203" s="2" t="s">
         <v>803</v>
       </c>
-      <c r="C203" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D203" s="5" t="s">
         <v>9</v>
       </c>
@@ -6882,7 +7071,7 @@
         <v>804</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>5</v>
+        <v>934</v>
       </c>
       <c r="D204" s="5" t="s">
         <v>9</v>
@@ -6898,9 +7087,6 @@
       <c r="B205" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C205" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D205" s="5" t="s">
         <v>7</v>
       </c>
@@ -6984,7 +7170,7 @@
         <v>805</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>5</v>
+        <v>935</v>
       </c>
       <c r="D210" s="5" t="s">
         <v>7</v>
@@ -7001,7 +7187,7 @@
         <v>793</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>5</v>
+        <v>936</v>
       </c>
       <c r="D211" s="5" t="s">
         <v>9</v>
@@ -7017,9 +7203,6 @@
       <c r="B212" s="2" t="s">
         <v>794</v>
       </c>
-      <c r="C212" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D212" s="5" t="s">
         <v>18</v>
       </c>
@@ -7035,7 +7218,7 @@
         <v>806</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>5</v>
+        <v>937</v>
       </c>
       <c r="D213" s="5" t="s">
         <v>7</v>
@@ -7052,7 +7235,7 @@
         <v>795</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>5</v>
+        <v>938</v>
       </c>
       <c r="D214" s="5" t="s">
         <v>9</v>
@@ -7086,7 +7269,7 @@
         <v>807</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>5</v>
+        <v>939</v>
       </c>
       <c r="D216" s="5" t="s">
         <v>10</v>
@@ -7103,7 +7286,7 @@
         <v>808</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>5</v>
+        <v>940</v>
       </c>
       <c r="D217" s="5" t="s">
         <v>7</v>
@@ -7137,7 +7320,7 @@
         <v>810</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>5</v>
+        <v>941</v>
       </c>
       <c r="G219" s="5" t="s">
         <v>116</v>
@@ -7151,7 +7334,7 @@
         <v>811</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>5</v>
+        <v>942</v>
       </c>
       <c r="D220" s="5" t="s">
         <v>9</v>
@@ -7202,7 +7385,7 @@
         <v>810</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>5</v>
+        <v>941</v>
       </c>
       <c r="D223" s="5" t="s">
         <v>7</v>
@@ -7219,7 +7402,7 @@
         <v>814</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>5</v>
+        <v>943</v>
       </c>
       <c r="D224" s="5" t="s">
         <v>7</v>
@@ -7270,7 +7453,7 @@
         <v>817</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>5</v>
+        <v>944</v>
       </c>
       <c r="D227" s="5" t="s">
         <v>9</v>
@@ -7386,10 +7569,10 @@
         <v>270</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>819</v>
+        <v>945</v>
       </c>
       <c r="C234" s="2" t="s">
-        <v>5</v>
+        <v>946</v>
       </c>
       <c r="D234" s="5" t="s">
         <v>17</v>
@@ -7403,7 +7586,7 @@
         <v>271</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C235" s="2" t="s">
         <v>5</v>
@@ -7420,10 +7603,10 @@
         <v>272</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>5</v>
+        <v>947</v>
       </c>
       <c r="D236" s="5" t="s">
         <v>9</v>
@@ -7437,10 +7620,10 @@
         <v>273</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>5</v>
+        <v>948</v>
       </c>
       <c r="D237" s="5" t="s">
         <v>7</v>
@@ -7454,10 +7637,10 @@
         <v>274</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>5</v>
+        <v>949</v>
       </c>
       <c r="D238" s="5" t="s">
         <v>7</v>
@@ -7471,10 +7654,10 @@
         <v>275</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>5</v>
+        <v>950</v>
       </c>
       <c r="D239" s="5" t="s">
         <v>14</v>
@@ -7488,10 +7671,10 @@
         <v>276</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>5</v>
+        <v>951</v>
       </c>
       <c r="D240" s="5" t="s">
         <v>7</v>
@@ -7505,7 +7688,7 @@
         <v>277</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C241" s="2" t="s">
         <v>5</v>
@@ -7522,10 +7705,10 @@
         <v>278</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>5</v>
+        <v>952</v>
       </c>
       <c r="D242" s="5" t="s">
         <v>19</v>
@@ -7539,10 +7722,10 @@
         <v>279</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>5</v>
+        <v>953</v>
       </c>
       <c r="D243" s="5" t="s">
         <v>19</v>
@@ -7556,7 +7739,7 @@
         <v>280</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C244" s="2" t="s">
         <v>5</v>
@@ -7570,10 +7753,10 @@
         <v>281</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>5</v>
+        <v>954</v>
       </c>
       <c r="D245" s="5" t="s">
         <v>16</v>
@@ -7587,10 +7770,10 @@
         <v>282</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>5</v>
+        <v>955</v>
       </c>
       <c r="D246" s="5" t="s">
         <v>7</v>
@@ -7604,10 +7787,10 @@
         <v>283</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>5</v>
+        <v>956</v>
       </c>
       <c r="D247" s="5" t="s">
         <v>7</v>
@@ -7621,10 +7804,10 @@
         <v>284</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C248" s="2" t="s">
-        <v>5</v>
+        <v>956</v>
       </c>
       <c r="D248" s="5" t="s">
         <v>7</v>
@@ -7638,10 +7821,10 @@
         <v>285</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>5</v>
+        <v>957</v>
       </c>
       <c r="D249" s="5" t="s">
         <v>16</v>
@@ -7655,10 +7838,10 @@
         <v>286</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>5</v>
+        <v>958</v>
       </c>
       <c r="D250" s="5" t="s">
         <v>7</v>
@@ -7672,10 +7855,10 @@
         <v>287</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>5</v>
+        <v>959</v>
       </c>
       <c r="D251" s="5" t="s">
         <v>7</v>
@@ -7689,10 +7872,10 @@
         <v>288</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>5</v>
+        <v>960</v>
       </c>
       <c r="D252" s="5" t="s">
         <v>7</v>
@@ -7706,10 +7889,10 @@
         <v>289</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>5</v>
+        <v>961</v>
       </c>
       <c r="D253" s="5" t="s">
         <v>18</v>
@@ -7723,10 +7906,10 @@
         <v>290</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>5</v>
+        <v>962</v>
       </c>
       <c r="D254" s="5" t="s">
         <v>7</v>
@@ -7740,10 +7923,10 @@
         <v>292</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C255" s="2" t="s">
-        <v>5</v>
+        <v>963</v>
       </c>
       <c r="D255" s="5" t="s">
         <v>7</v>
@@ -7757,7 +7940,7 @@
         <v>293</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="C256" s="2" t="s">
         <v>5</v>
@@ -7771,7 +7954,7 @@
         <v>294</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C257" s="2" t="s">
         <v>5</v>
@@ -7788,10 +7971,10 @@
         <v>295</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C258" s="2" t="s">
-        <v>5</v>
+        <v>964</v>
       </c>
       <c r="D258" s="5" t="s">
         <v>9</v>
@@ -7813,7 +7996,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>